<commit_message>
RM-110 Beheer->Interface scherm klaar
</commit_message>
<xml_diff>
--- a/rm/test/resources/a_valid_excel_file.xlsx
+++ b/rm/test/resources/a_valid_excel_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t xml:space="preserve">Database nr.</t>
   </si>
@@ -106,22 +106,28 @@
     <t xml:space="preserve">Lopend contract</t>
   </si>
   <si>
-    <t xml:space="preserve">Maandelijkse Facturatie a €221,34I = geschatte éénmalige investeringskosten n.v.t.Y = aantal jaren looptijd overeenkomstX = geschatte jaarlijkse kosten</t>
+    <t xml:space="preserve">Maandelijkse Facturatie a 500 Gulden</t>
   </si>
   <si>
     <t xml:space="preserve">NPO/Technology/IAAS</t>
   </si>
   <si>
-    <t xml:space="preserve">Bart Adriaanse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bart.adriaanse@npo.nl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">035 677 8899</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KRO-NCRV(AKN)-mw/0211/016 Colo remote extra 1 Gb koppeling</t>
+    <t xml:space="preserve">Boris Dietrich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b.dietrich@npo.nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06-654654654</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06-654654</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Circustent Boltini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPO/Technology/Data Services</t>
   </si>
 </sst>
 </file>
@@ -214,7 +220,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -233,10 +239,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -256,13 +258,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -344,7 +346,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -381,7 +383,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="4" t="n">
-        <v>2656</v>
+        <v>2500</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2" t="s">
@@ -391,67 +393,78 @@
         <v>31</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>567567</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>567567</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>44256.4583333333</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="4" t="n">
+        <v>2500</v>
+      </c>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="b.dietrich@npo.nl"/>
+    <hyperlink ref="U2" r:id="rId2" display="b.dietrich@npo.nl"/>
+    <hyperlink ref="H3" r:id="rId3" display="b.dietrich@npo.nl"/>
+    <hyperlink ref="U3" r:id="rId4" display="b.dietrich@npo.nl"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>